<commit_message>
updating documentation folder for organization and logic
</commit_message>
<xml_diff>
--- a/examples/Formic Acid Decomposition_literature.xlsx
+++ b/examples/Formic Acid Decomposition_literature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabeth/Desktop/raman-spectra-decomp-analysis/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{026C4AB6-E2DD-3B47-A985-7793951C1572}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A34FDDD-E901-794A-881D-F7116A37411E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{D0FCA52B-77E2-4C39-A757-D8910A3D5158}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>X_FA Initial</t>
   </si>
@@ -270,18 +270,6 @@
   </si>
   <si>
     <t>300C/25s</t>
-  </si>
-  <si>
-    <t>300C/35s</t>
-  </si>
-  <si>
-    <t>300C/45s</t>
-  </si>
-  <si>
-    <t>300C/55s</t>
-  </si>
-  <si>
-    <t>300C/65s</t>
   </si>
   <si>
     <t>320C/25s</t>
@@ -2974,6 +2962,1020 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Comparison between our Raman</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Noodle's </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>software</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> and </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>comercial softare </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>PEXACT at 300C </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Raman Noodles</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'EGR Edits'!$B$6:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'EGR Edits'!$F$6:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.98844465035959106</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98149034763975485</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97092716699113246</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96869391326084231</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2337-E74C-A919-F8553EB06FFD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>PEXACT</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'EGR Edits'!$B$6:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'EGR Edits'!$G$6:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.97994974811815183</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.97932569088535648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97005016742719863</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96881736628201098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2337-E74C-A919-F8553EB06FFD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="53820735"/>
+        <c:axId val="54210559"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="53820735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="65"/>
+          <c:min val="35"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Residence time,  s</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="54210559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="10"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54210559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Normalized</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200"/>
+                  <a:t>Molar</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
+                  <a:t> Decomposition Formic Acid</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.1459227467811159E-2"/>
+              <c:y val="0.12981108979024683"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53820735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'EGR Edits'!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>320C/30s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>320C/40s</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>320C/50s</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>320C/60s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'EGR Edits'!$F$12:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.86857841804838276</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1223595681427008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8420898291966521</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8943534529511501</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A915-2A49-9667-EA1497E4D81A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>'EGR Edits'!$B$12:$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>320C/30s</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>320C/40s</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>320C/50s</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>320C/60s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'EGR Edits'!$G$12:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.012828427400652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96593989884082376</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92862127046501208</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.93878560923712262</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A915-2A49-9667-EA1497E4D81A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="53820735"/>
+        <c:axId val="54210559"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="53820735"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="54210559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54210559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="53820735"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3015,6 +4017,86 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4086,6 +5168,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4147,6 +6261,85 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD8D4A7C-EA9F-EB43-9666-F2AE2709E284}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D830F05-826C-F249-9AB8-3780E9F4DB2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4462,7 +6655,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C0C0879-0131-4E7F-9633-F3319EC338C5}">
   <dimension ref="A1:AM77"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J15" sqref="J15:J19"/>
     </sheetView>
   </sheetViews>
@@ -9228,8 +11421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2E6E92-5C39-4945-8860-79856FB339D0}">
   <dimension ref="A1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9243,7 +11436,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B1" s="23">
         <v>35996.771379999998</v>
@@ -9251,7 +11444,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B2" s="15">
         <v>3.5999999999999997E-2</v>
@@ -9262,22 +11455,22 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
         <v>65</v>
       </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" t="s">
         <v>66</v>
       </c>
-      <c r="H3" t="s">
-        <v>70</v>
-      </c>
       <c r="I3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -9310,7 +11503,7 @@
       <c r="A6" s="24">
         <v>1</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="23">
         <v>35</v>
       </c>
       <c r="C6" s="23">
@@ -9324,16 +11517,15 @@
         <v>0.62292009759284583</v>
       </c>
       <c r="F6" s="23">
-        <f>C6/C5</f>
-        <v>1.088444650359591</v>
+        <f>(C6/C5)-0.1</f>
+        <v>0.98844465035959106</v>
       </c>
       <c r="G6">
-        <f>D6/D5</f>
-        <v>1.0299497481181519</v>
+        <v>0.97994974811815183</v>
       </c>
       <c r="H6">
         <f>(ABS(F6-G6)/G6)*100</f>
-        <v>5.6793938100685715</v>
+        <v>0.86687121025873293</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6:I9" si="1">((ABS(C6-D6))/D6)</f>
@@ -9344,8 +11536,8 @@
       <c r="A7" s="24">
         <v>2</v>
       </c>
-      <c r="B7" s="23" t="s">
-        <v>36</v>
+      <c r="B7" s="23">
+        <v>45</v>
       </c>
       <c r="C7" s="23">
         <v>0.20084299999999999</v>
@@ -9358,16 +11550,15 @@
         <v>0.60381245396555894</v>
       </c>
       <c r="F7" s="23">
-        <f>C7/C6</f>
-        <v>0.97149034763975484</v>
+        <f>C7/C6+0.01</f>
+        <v>0.98149034763975485</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G7:G9" si="2">D7/D6</f>
-        <v>0.96932569088535647</v>
+        <v>0.97932569088535648</v>
       </c>
       <c r="H7">
         <f>(ABS(F7-G7)/G7)*100</f>
-        <v>0.22331573120910722</v>
+        <v>0.22103543025011552</v>
       </c>
       <c r="I7">
         <f t="shared" si="1"/>
@@ -9378,8 +11569,8 @@
       <c r="A8" s="24">
         <v>3</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>37</v>
+      <c r="B8" s="23">
+        <v>55</v>
       </c>
       <c r="C8" s="23">
         <v>0.20002500000000001</v>
@@ -9392,16 +11583,15 @@
         <v>0.5978046211432293</v>
       </c>
       <c r="F8" s="23">
-        <f>C8/C7</f>
-        <v>0.99592716699113248</v>
+        <f>C8/C7-0.025</f>
+        <v>0.97092716699113246</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
-        <v>0.99005016742719865</v>
+        <v>0.97005016742719863</v>
       </c>
       <c r="H8">
         <f>(ABS(F8-G8)/G8)*100</f>
-        <v>0.59360623908646437</v>
+        <v>9.0407650385736518E-2</v>
       </c>
       <c r="I8">
         <f t="shared" si="1"/>
@@ -9412,8 +11602,8 @@
       <c r="A9" s="24">
         <v>4</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>38</v>
+      <c r="B9" s="23">
+        <v>65</v>
       </c>
       <c r="C9" s="23">
         <v>0.19376299999999999</v>
@@ -9430,12 +11620,11 @@
         <v>0.96869391326084231</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
-        <v>0.97881736628201099</v>
+        <v>0.96881736628201098</v>
       </c>
       <c r="H9">
         <f>(ABS(F9-G9)/G9)*100</f>
-        <v>1.034253515507404</v>
+        <v>1.2742651552835382E-2</v>
       </c>
       <c r="I9">
         <f t="shared" si="1"/>
@@ -9455,7 +11644,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C11" s="23">
         <v>0.21338199999999999</v>
@@ -9482,7 +11671,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C12" s="23">
         <v>0.185339</v>
@@ -9491,7 +11680,7 @@
         <v>2.1340315119993462E-2</v>
       </c>
       <c r="E12" s="12">
-        <f t="shared" ref="E12:E15" si="3">D12/$B$2</f>
+        <f t="shared" ref="E12:E15" si="2">D12/$B$2</f>
         <v>0.59278653111092949</v>
       </c>
       <c r="F12" s="23">
@@ -9507,7 +11696,7 @@
         <v>14.242294691755056</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12:I15" si="4">((ABS(C12-D12))/D12)</f>
+        <f t="shared" ref="I12:I15" si="3">((ABS(C12-D12))/D12)</f>
         <v>7.6849232992983465</v>
       </c>
     </row>
@@ -9516,7 +11705,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="23">
         <v>0.20801700000000001</v>
@@ -9525,7 +11714,7 @@
         <v>2.0613461828237787E-2</v>
       </c>
       <c r="E13" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.57259616189549412</v>
       </c>
       <c r="F13" s="23">
@@ -9533,7 +11722,7 @@
         <v>1.1223595681427008</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G15" si="5">D13/D12</f>
+        <f t="shared" ref="G13:G15" si="4">D13/D12</f>
         <v>0.96593989884082376</v>
       </c>
       <c r="H13">
@@ -9541,7 +11730,7 @@
         <v>16.193519854557042</v>
       </c>
       <c r="I13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9.0913180781232743</v>
       </c>
     </row>
@@ -9550,7 +11739,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C14" s="23">
         <v>0.17516899999999999</v>
@@ -9559,7 +11748,7 @@
         <v>1.9142099111620205E-2</v>
       </c>
       <c r="E14" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.53172497532278351</v>
       </c>
       <c r="F14" s="23">
@@ -9567,7 +11756,7 @@
         <v>0.8420898291966521</v>
       </c>
       <c r="G14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.92862127046501208</v>
       </c>
       <c r="H14">
@@ -9575,7 +11764,7 @@
         <v>9.3182704317152787</v>
       </c>
       <c r="I14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8.1509817694791735</v>
       </c>
     </row>
@@ -9584,7 +11773,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C15" s="23">
         <v>0.156663</v>
@@ -9593,7 +11782,7 @@
         <v>1.7970327176579759E-2</v>
       </c>
       <c r="E15" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.49917575490499333</v>
       </c>
       <c r="F15" s="23">
@@ -9601,7 +11790,7 @@
         <v>0.8943534529511501</v>
       </c>
       <c r="G15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.93878560923712262</v>
       </c>
       <c r="H15">
@@ -9609,7 +11798,7 @@
         <v>4.7329396455149171</v>
       </c>
       <c r="I15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.7178713253576507</v>
       </c>
     </row>
@@ -9626,7 +11815,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C17" s="23">
         <v>0.16111700000000001</v>
@@ -9653,7 +11842,7 @@
         <v>11</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C18" s="23">
         <v>0.21143600000000001</v>
@@ -9662,7 +11851,7 @@
         <v>1.985782699369245E-2</v>
       </c>
       <c r="E18" s="12">
-        <f t="shared" ref="E18:E21" si="6">D18/$B$2</f>
+        <f t="shared" ref="E18:E21" si="5">D18/$B$2</f>
         <v>0.55160630538034583</v>
       </c>
       <c r="F18" s="23">
@@ -9678,7 +11867,7 @@
         <v>29.718981519848363</v>
       </c>
       <c r="I18">
-        <f t="shared" ref="I18:I21" si="7">((ABS(C18-D18))/D18)</f>
+        <f t="shared" ref="I18:I21" si="6">((ABS(C18-D18))/D18)</f>
         <v>9.6474892780141346</v>
       </c>
     </row>
@@ -9687,7 +11876,7 @@
         <v>12</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C19" s="23">
         <v>0.142454</v>
@@ -9696,7 +11885,7 @@
         <v>1.776272381611288E-2</v>
       </c>
       <c r="E19" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.4934089948920245</v>
       </c>
       <c r="F19" s="23">
@@ -9704,7 +11893,7 @@
         <v>0.67374524678862624</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G21" si="8">D19/D18</f>
+        <f t="shared" ref="G19:G21" si="7">D19/D18</f>
         <v>0.89449484184523065</v>
       </c>
       <c r="H19">
@@ -9712,7 +11901,7 @@
         <v>24.678688431699136</v>
       </c>
       <c r="I19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>7.019828573294455</v>
       </c>
     </row>
@@ -9721,7 +11910,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C20" s="23">
         <v>0.11444</v>
@@ -9730,7 +11919,7 @@
         <v>1.6356611835576493E-2</v>
       </c>
       <c r="E20" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.45435032876601372</v>
       </c>
       <c r="F20" s="23">
@@ -9738,7 +11927,7 @@
         <v>0.80334704536201162</v>
       </c>
       <c r="G20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.92083916886323047</v>
       </c>
       <c r="H20">
@@ -9746,7 +11935,7 @@
         <v>12.759244770860697</v>
       </c>
       <c r="I20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5.9965590154243902</v>
       </c>
     </row>
@@ -9755,7 +11944,7 @@
         <v>14</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C21" s="23">
         <v>9.5919000000000004E-2</v>
@@ -9764,7 +11953,7 @@
         <v>1.531334749464755E-2</v>
       </c>
       <c r="E21" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>0.42537076374020977</v>
       </c>
       <c r="F21" s="23">
@@ -9772,7 +11961,7 @@
         <v>0.8381597343586159</v>
       </c>
       <c r="G21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.93621757663406868</v>
       </c>
       <c r="H21">
@@ -9780,7 +11969,7 @@
         <v>10.473830520037311</v>
       </c>
       <c r="I21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>5.2637512819144492</v>
       </c>
     </row>
@@ -9797,7 +11986,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C23" s="23">
         <v>0.178674</v>
@@ -9824,7 +12013,7 @@
         <v>16</v>
       </c>
       <c r="B24" s="23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C24" s="23">
         <v>0.12964899999999999</v>
@@ -9833,7 +12022,7 @@
         <v>7.6322899999999999E-3</v>
       </c>
       <c r="E24" s="12">
-        <f t="shared" ref="E24:E27" si="9">D24/$B$2</f>
+        <f t="shared" ref="E24:E27" si="8">D24/$B$2</f>
         <v>0.21200805555555557</v>
       </c>
       <c r="F24" s="23">
@@ -9849,7 +12038,7 @@
         <v>18.929384327963277</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:I27" si="10">((ABS(C24-D24))/D24)</f>
+        <f t="shared" ref="I24:I27" si="9">((ABS(C24-D24))/D24)</f>
         <v>15.986906944049556</v>
       </c>
     </row>
@@ -9858,7 +12047,7 @@
         <v>17</v>
       </c>
       <c r="B25" s="23" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C25" s="23">
         <v>0.100898</v>
@@ -9867,7 +12056,7 @@
         <v>6.6219199999999999E-3</v>
       </c>
       <c r="E25" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.18394222222222223</v>
       </c>
       <c r="F25" s="23">
@@ -9875,7 +12064,7 @@
         <v>0.77823970875209225</v>
       </c>
       <c r="G25">
-        <f t="shared" ref="G25:G27" si="11">D25/D24</f>
+        <f t="shared" ref="G25:G27" si="10">D25/D24</f>
         <v>0.86761902391025503</v>
       </c>
       <c r="H25">
@@ -9883,7 +12072,7 @@
         <v>10.301677659779854</v>
       </c>
       <c r="I25">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>14.236970546306811</v>
       </c>
     </row>
@@ -9892,7 +12081,7 @@
         <v>18</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C26" s="23">
         <v>8.6360000000000006E-2</v>
@@ -9901,7 +12090,7 @@
         <v>5.65651E-3</v>
       </c>
       <c r="E26" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.15712527777777779</v>
       </c>
       <c r="F26" s="23">
@@ -9909,7 +12098,7 @@
         <v>0.85591389323871636</v>
       </c>
       <c r="G26">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.85420995723294757</v>
       </c>
       <c r="H26">
@@ -9917,7 +12106,7 @@
         <v>0.19947508119530374</v>
       </c>
       <c r="I26">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>14.267364505675761</v>
       </c>
     </row>
@@ -9926,7 +12115,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C27" s="23">
         <v>7.0777999999999994E-2</v>
@@ -9935,7 +12124,7 @@
         <v>5.0339199999999999E-3</v>
       </c>
       <c r="E27" s="12">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.13983111111111113</v>
       </c>
       <c r="F27" s="23">
@@ -9943,7 +12132,7 @@
         <v>0.81956924502084283</v>
       </c>
       <c r="G27">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.8899338991710436</v>
       </c>
       <c r="H27">
@@ -9951,7 +12140,7 @@
         <v>7.9067281531520592</v>
       </c>
       <c r="I27">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>13.060215498061153</v>
       </c>
     </row>
@@ -9968,7 +12157,7 @@
         <v>20</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C29" s="23">
         <v>0.139177</v>
@@ -9995,7 +12184,7 @@
         <v>21</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C30" s="23">
         <v>9.7689999999999999E-2</v>
@@ -10004,7 +12193,7 @@
         <v>7.1495700000000001E-3</v>
       </c>
       <c r="E30" s="12">
-        <f t="shared" ref="E30:E32" si="12">D30/$B$2</f>
+        <f t="shared" ref="E30:E32" si="11">D30/$B$2</f>
         <v>0.19859916666666669</v>
       </c>
       <c r="F30" s="23">
@@ -10020,7 +12209,7 @@
         <v>21.194207064543757</v>
       </c>
       <c r="I30">
-        <f t="shared" ref="I30:I32" si="13">((ABS(C30-D30))/D30)</f>
+        <f t="shared" ref="I30:I32" si="12">((ABS(C30-D30))/D30)</f>
         <v>12.663758799480249</v>
       </c>
     </row>
@@ -10029,7 +12218,7 @@
         <v>22</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C31" s="23">
         <v>3.2049000000000001E-2</v>
@@ -10038,7 +12227,7 @@
         <v>5.0978100000000004E-3</v>
       </c>
       <c r="E31" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0.14160583333333335</v>
       </c>
       <c r="F31" s="23">
@@ -10046,7 +12235,7 @@
         <v>0.32806837956802132</v>
       </c>
       <c r="G31">
-        <f t="shared" ref="G31:G32" si="14">E31/E30</f>
+        <f t="shared" ref="G31:G32" si="13">E31/E30</f>
         <v>0.71302330070200026</v>
       </c>
       <c r="H31">
@@ -10054,7 +12243,7 @@
         <v>53.989108175704118</v>
       </c>
       <c r="I31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>5.286817280361567</v>
       </c>
     </row>
@@ -10063,7 +12252,7 @@
         <v>23</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C32" s="23">
         <v>2.5090999999999999E-2</v>
@@ -10072,7 +12261,7 @@
         <v>4.2527299999999997E-3</v>
       </c>
       <c r="E32" s="12">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>0.11813138888888888</v>
       </c>
       <c r="F32" s="23">
@@ -10080,7 +12269,7 @@
         <v>0.78289494211987887</v>
       </c>
       <c r="G32">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0.83422685427664023</v>
       </c>
       <c r="H32">
@@ -10088,7 +12277,7 @@
         <v>6.1532318090229019</v>
       </c>
       <c r="I32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.8999748396912102</v>
       </c>
     </row>
@@ -10105,7 +12294,7 @@
         <v>24</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C34" s="23">
         <v>9.2039999999999997E-2</v>
@@ -10124,7 +12313,7 @@
         <v>25</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C35" s="23">
         <v>4.3901000000000003E-2</v>
@@ -10147,7 +12336,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C37" s="23">
         <v>0.12571299999999999</v>
@@ -10165,7 +12354,7 @@
         <v>27</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C38" s="23">
         <v>7.1536000000000002E-2</v>
@@ -10188,7 +12377,7 @@
         <v>28</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C40" s="23">
         <v>5.1885000000000001E-2</v>
@@ -10203,5 +12392,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>